<commit_message>
extract data only from 2024 and remove unnecessary data
</commit_message>
<xml_diff>
--- a/Separate_Data/World_Happiness_Report_from_2011_to_2024.xlsx
+++ b/Separate_Data/World_Happiness_Report_from_2011_to_2024.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Main_Directory\Random_Stuff\Countries_Data_Analysis\Separate_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BC5F50-CF29-481E-B854-00DF348A95AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F171F28-9FEB-4944-976C-40CBB2FB95DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="world-happieness-report" sheetId="1" r:id="rId1"/>
+    <sheet name="world-happieness-report-2024" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="181">
   <si>
     <t>Year</t>
   </si>
@@ -644,7 +658,64 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -655,6 +726,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D300515-02B6-4C4E-9A9F-B8CF79B76AA6}" name="Tabelle2" displayName="Tabelle2" ref="A1:C148" totalsRowShown="0">
+  <autoFilter ref="A1:C148" xr:uid="{3D300515-02B6-4C4E-9A9F-B8CF79B76AA6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C148">
+    <sortCondition ref="A1:A148"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="2" xr3:uid="{884DEEC0-6F7D-4A4E-B494-09C6F1FBDF7F}" name="Rank" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{A55D094B-1831-46FE-B9B8-250201EC6E2C}" name="Country name" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{9DDB04D2-CC07-40C6-B4A4-3FF930E9CFB0}" name="Life evaluation (3-year average)" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -860,9 +946,9 @@
   </sheetPr>
   <dimension ref="A1:AB2625"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="C1940" sqref="C1940"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -71736,4 +71822,1654 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF102AF-4F95-4DDB-BBA4-C75F71DB4A1A}">
+  <dimension ref="A1:C148"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="30.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="7">
+        <v>7.7359999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="7">
+        <v>7.5209999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="7">
+        <v>7.5149999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="7">
+        <v>7.3449999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="7">
+        <v>7.306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="7">
+        <v>7.274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="7">
+        <v>7.2619999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="7">
+        <v>7.234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="7">
+        <v>7.1219999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="7">
+        <v>6.9790000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="7">
+        <v>6.9740000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="7">
+        <v>6.952</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" s="7">
+        <v>6.9349999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="7">
+        <v>6.91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="7">
+        <v>6.8890000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="7">
+        <v>6.8289999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="7">
+        <v>6.81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="7">
+        <v>6.8029999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" s="7">
+        <v>6.7919999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="7">
+        <v>6.7750000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="7">
+        <v>6.7590000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="7">
+        <v>6.7530000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" s="7">
+        <v>6.7279999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" s="7">
+        <v>6.7240000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="7">
+        <v>6.7110000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" s="7">
+        <v>6.673</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28" s="7">
+        <v>6.6689999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="7">
+        <v>6.6609999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="7">
+        <v>6.6589999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="7">
+        <v>6.6289999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="7">
+        <v>6.6059999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" s="7">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="7">
+        <v>6.593</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C35" s="7">
+        <v>6.5650000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" s="7">
+        <v>6.5629999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="7">
+        <v>6.4939999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="7">
+        <v>6.492</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="7">
+        <v>6.4660000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="7">
+        <v>6.4169999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="7">
+        <v>6.415</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C42" s="7">
+        <v>6.407</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="7">
+        <v>6.3970000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="7">
+        <v>6.3780000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="7">
+        <v>6.3620000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="7">
+        <v>6.3609999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" s="7">
+        <v>6.3520000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="7">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="7">
+        <v>6.3159999999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C50" s="7">
+        <v>6.2220000000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <v>50</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="7">
+        <v>6.2210000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="7">
+        <v>6.2069999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="5">
+        <v>52</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="7">
+        <v>6.1970000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
+        <v>53</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C54" s="7">
+        <v>6.1929999999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
+        <v>54</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="7">
+        <v>6.1719999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="7">
+        <v>6.1470000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
+        <v>56</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="7">
+        <v>6.1360000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <v>57</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C58" s="7">
+        <v>6.1070000000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <v>58</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59" s="7">
+        <v>6.0380000000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="7">
+        <v>6.03</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
+        <v>60</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" s="7">
+        <v>6.0129999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" s="7">
+        <v>6.0039999999999996</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="5">
+        <v>62</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" s="7">
+        <v>5.9649999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" s="7">
+        <v>5.9640000000000004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>64</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C65" s="7">
+        <v>5.9550000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="7">
+        <v>5.9470000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
+        <v>66</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" s="7">
+        <v>5.9450000000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C68" s="7">
+        <v>5.9420000000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="5">
+        <v>68</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C69" s="7">
+        <v>5.9210000000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="5">
+        <v>69</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" s="7">
+        <v>5.915</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>70</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" s="7">
+        <v>5.9050000000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
+        <v>71</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C72" s="7">
+        <v>5.8769999999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>72</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C73" s="7">
+        <v>5.87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="5">
+        <v>73</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C74" s="7">
+        <v>5.87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="5">
+        <v>74</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C75" s="7">
+        <v>5.8680000000000003</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="5">
+        <v>75</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C76" s="7">
+        <v>5.8579999999999997</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
+        <v>76</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C77" s="7">
+        <v>5.8460000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="5">
+        <v>77</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C78" s="7">
+        <v>5.8330000000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="5">
+        <v>78</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C79" s="7">
+        <v>5.8319999999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="5">
+        <v>79</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C80" s="7">
+        <v>5.82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="5">
+        <v>80</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C81" s="7">
+        <v>5.819</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="5">
+        <v>81</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C82" s="7">
+        <v>5.7759999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="5">
+        <v>82</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C83" s="7">
+        <v>5.6829999999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="5">
+        <v>83</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C84" s="7">
+        <v>5.617</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="5">
+        <v>84</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="7">
+        <v>5.5709999999999997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="5">
+        <v>85</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C86" s="7">
+        <v>5.5540000000000003</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="5">
+        <v>86</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C87" s="7">
+        <v>5.5030000000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="5">
+        <v>87</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C88" s="7">
+        <v>5.4939999999999998</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="5">
+        <v>88</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C89" s="7">
+        <v>5.4909999999999997</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="5">
+        <v>89</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="7">
+        <v>5.4109999999999996</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="5">
+        <v>90</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C91" s="7">
+        <v>5.4109999999999996</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
+        <v>91</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C92" s="7">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="5">
+        <v>92</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C93" s="7">
+        <v>5.3109999999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="5">
+        <v>93</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C94" s="7">
+        <v>5.3010000000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="5">
+        <v>94</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C95" s="7">
+        <v>5.2619999999999996</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="5">
+        <v>95</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C96" s="7">
+        <v>5.2130000000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
+        <v>96</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C97" s="7">
+        <v>5.19</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="5">
+        <v>97</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C98" s="7">
+        <v>5.12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="5">
+        <v>98</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C99" s="7">
+        <v>5.1020000000000003</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="5">
+        <v>99</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C100" s="7">
+        <v>5.093</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="5">
+        <v>100</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C101" s="7">
+        <v>5.03</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="5">
+        <v>101</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C102" s="7">
+        <v>4.976</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="5">
+        <v>102</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C103" s="7">
+        <v>4.9290000000000003</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="5">
+        <v>103</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C104" s="7">
+        <v>4.9109999999999996</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="5">
+        <v>104</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C105" s="7">
+        <v>4.8869999999999996</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="5">
+        <v>105</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C106" s="7">
+        <v>4.8849999999999998</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="5">
+        <v>106</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C107" s="7">
+        <v>4.875</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="5">
+        <v>107</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C108" s="7">
+        <v>4.8559999999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="5">
+        <v>108</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C109" s="7">
+        <v>4.78</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="5">
+        <v>109</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C110" s="7">
+        <v>4.7679999999999998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="5">
+        <v>110</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C111" s="7">
+        <v>4.7249999999999996</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="5">
+        <v>111</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C112" s="7">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="5">
+        <v>112</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C113" s="7">
+        <v>4.6219999999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="5">
+        <v>113</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C114" s="7">
+        <v>4.5519999999999996</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="5">
+        <v>114</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C115" s="7">
+        <v>4.5419999999999998</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="5">
+        <v>115</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C116" s="7">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="5">
+        <v>116</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C117" s="7">
+        <v>4.4610000000000003</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="5">
+        <v>117</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C118" s="7">
+        <v>4.423</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="5">
+        <v>118</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C119" s="7">
+        <v>4.3890000000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="5">
+        <v>119</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C120" s="7">
+        <v>4.3840000000000003</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="5">
+        <v>120</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C121" s="7">
+        <v>4.383</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="5">
+        <v>121</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C122" s="7">
+        <v>4.3570000000000002</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="5">
+        <v>122</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C123" s="7">
+        <v>4.3470000000000004</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="5">
+        <v>123</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C124" s="7">
+        <v>4.3449999999999998</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="5">
+        <v>124</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C125" s="7">
+        <v>4.3410000000000002</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="5">
+        <v>125</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C126" s="7">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="5">
+        <v>126</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C127" s="7">
+        <v>4.3209999999999997</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="5">
+        <v>127</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C128" s="7">
+        <v>4.3150000000000004</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="5">
+        <v>128</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C129" s="7">
+        <v>4.3099999999999996</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="5">
+        <v>129</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C130" s="7">
+        <v>4.2770000000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="5">
+        <v>130</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C131" s="7">
+        <v>4.157</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="5">
+        <v>131</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C132" s="7">
+        <v>3.9119999999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="5">
+        <v>132</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C133" s="7">
+        <v>3.8980000000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="5">
+        <v>133</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C134" s="7">
+        <v>3.891</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="5">
+        <v>134</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C135" s="7">
+        <v>3.851</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="5">
+        <v>135</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C136" s="7">
+        <v>3.8170000000000002</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="5">
+        <v>136</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C137" s="7">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="5">
+        <v>137</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C138" s="7">
+        <v>3.774</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="5">
+        <v>138</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C139" s="7">
+        <v>3.7570000000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="5">
+        <v>139</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C140" s="7">
+        <v>3.754</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="5">
+        <v>140</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C141" s="7">
+        <v>3.5609999999999999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="5">
+        <v>141</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C142" s="7">
+        <v>3.4689999999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="5">
+        <v>142</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C143" s="7">
+        <v>3.4380000000000002</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="5">
+        <v>143</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C144" s="7">
+        <v>3.3959999999999999</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="5">
+        <v>144</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C145" s="7">
+        <v>3.26</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="5">
+        <v>145</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C146" s="7">
+        <v>3.1880000000000002</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="5">
+        <v>146</v>
+      </c>
+      <c r="B147" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C147" s="7">
+        <v>2.9980000000000002</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="5">
+        <v>147</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C148" s="7">
+        <v>1.3640000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>